<commit_message>
622 : passage au vert !
53%
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles en 2017.xlsx
+++ b/Src/622 miles/Objectif 622 miles en 2017.xlsx
@@ -882,11 +882,12 @@
         <v>18</v>
       </c>
       <c r="I6" s="2">
-        <v>7.26</v>
+        <f>+ 7.26 + 7.55</f>
+        <v>14.809999999999999</v>
       </c>
       <c r="J6" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>539.95000000000005</v>
+        <v>547.5</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="11">
@@ -1201,7 +1202,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="11">
         <f ca="1">MAX(J3:J12)</f>
-        <v>539.95000000000005</v>
+        <v>547.5</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -1214,7 +1215,7 @@
       </c>
       <c r="I16" s="14">
         <f ca="1">1 - $H$18/$H$17</f>
-        <v>0.47815302423201711</v>
+        <v>0.5261718501558228</v>
       </c>
     </row>
     <row r="17" spans="8:9" x14ac:dyDescent="0.25">
@@ -1229,11 +1230,11 @@
     <row r="18" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H18" s="12">
         <f ca="1">622-$J$13</f>
-        <v>82.049999999999955</v>
+        <v>74.5</v>
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43053</v>
+        <v>43054</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
622 ... à 9%
91% !
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles en 2017.xlsx
+++ b/Src/622 miles/Objectif 622 miles en 2017.xlsx
@@ -985,12 +985,12 @@
         <v>18</v>
       </c>
       <c r="I8" s="2">
-        <f xml:space="preserve"> 6.19</f>
-        <v>6.19</v>
+        <f xml:space="preserve"> 6.19 + 6.19</f>
+        <v>12.38</v>
       </c>
       <c r="J8" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>601.04000000000019</v>
+        <v>607.23000000000013</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="11">
@@ -1208,7 +1208,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="11">
         <f ca="1">MAX(J3:J12)</f>
-        <v>601.04000000000019</v>
+        <v>607.23000000000013</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="I16" s="14">
         <f ca="1">1 - $H$18/$H$17</f>
-        <v>0.86669210710424349</v>
+        <v>0.90606118425237003</v>
       </c>
     </row>
     <row r="17" spans="8:9" x14ac:dyDescent="0.25">
@@ -1236,11 +1236,11 @@
     <row r="18" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H18" s="12">
         <f ca="1">622-$J$13</f>
-        <v>20.959999999999809</v>
+        <v>14.769999999999868</v>
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43066</v>
+        <v>43067</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
622 .... done !
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles en 2017.xlsx
+++ b/Src/622 miles/Objectif 622 miles en 2017.xlsx
@@ -985,12 +985,12 @@
         <v>18</v>
       </c>
       <c r="I8" s="2">
-        <f xml:space="preserve"> 6.19 + 6.19 + 6.76</f>
-        <v>19.14</v>
+        <f xml:space="preserve"> 6.19 + 6.19 + 6.76 + 8.47</f>
+        <v>27.61</v>
       </c>
       <c r="J8" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>613.99000000000012</v>
+        <v>622.46000000000015</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="11">
@@ -1208,7 +1208,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="11">
         <f ca="1">MAX(J3:J12)</f>
-        <v>613.99000000000012</v>
+        <v>622.46000000000015</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="I16" s="14">
         <f ca="1">1 - $H$18/$H$17</f>
-        <v>0.94905552375500934</v>
+        <v>1.0029256503211865</v>
       </c>
     </row>
     <row r="17" spans="8:9" x14ac:dyDescent="0.25">
@@ -1236,11 +1236,11 @@
     <row r="18" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H18" s="12">
         <f ca="1">622-$J$13</f>
-        <v>8.0099999999998772</v>
+        <v>-0.46000000000015007</v>
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43068</v>
+        <v>43070</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nous frisons les 3/4
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles en 2017.xlsx
+++ b/Src/622 miles/Objectif 622 miles en 2017.xlsx
@@ -1659,7 +1659,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43317</v>
+        <v>43319</v>
       </c>
     </row>
   </sheetData>
@@ -1792,7 +1792,7 @@
       <pane xSplit="11" ySplit="3" topLeftCell="L32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J39" sqref="J39"/>
+      <selection pane="bottomRight" activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1843,12 +1843,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>459.09</v>
+        <v>466.26</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.73808681672025722</v>
+        <v>0.74961414790996783</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -3284,7 +3284,10 @@
         <f t="shared" si="42"/>
         <v>43324</v>
       </c>
-      <c r="J40" s="24"/>
+      <c r="J40" s="24">
+        <f xml:space="preserve"> 7.17</f>
+        <v>7.17</v>
+      </c>
       <c r="K40" s="24"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -3395,7 +3398,7 @@
       <c r="J43" s="24"/>
       <c r="K43" s="24">
         <f>SUM(J40:J43)</f>
-        <v>0</v>
+        <v>7.17</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Dans le mille !
Et au delà !
</commit_message>
<xml_diff>
--- a/Src/622 miles/Objectif 622 miles en 2017.xlsx
+++ b/Src/622 miles/Objectif 622 miles en 2017.xlsx
@@ -15,7 +15,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2018'!$B$3:$H$3</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1659,7 +1659,7 @@
       </c>
       <c r="I18" s="13">
         <f ca="1">TODAY()</f>
-        <v>43394</v>
+        <v>43400</v>
       </c>
     </row>
   </sheetData>
@@ -1792,7 +1792,7 @@
       <pane xSplit="11" ySplit="3" topLeftCell="L32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J50" sqref="J50"/>
+      <selection pane="bottomRight" activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1843,12 +1843,12 @@
       </c>
       <c r="J3" s="25">
         <f>SUM($J$4:$J$61)</f>
-        <v>619.06000000000006</v>
+        <v>628.20000000000005</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="27">
         <f xml:space="preserve"> J3 / 622</f>
-        <v>0.99527331189710622</v>
+        <v>1.0099678456591641</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -3719,7 +3719,9 @@
         <f t="shared" si="55"/>
         <v>43401</v>
       </c>
-      <c r="J51" s="24"/>
+      <c r="J51" s="24">
+        <v>9.14</v>
+      </c>
       <c r="K51" s="24"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -3758,7 +3760,7 @@
       <c r="J52" s="24"/>
       <c r="K52" s="24">
         <f>SUM(J48:J52)</f>
-        <v>48.179999999999993</v>
+        <v>57.319999999999993</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>